<commit_message>
Updated map according to new data
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\97254\Desktop\Guy\Projects\Rentalytics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0447ACE-F424-4B18-B904-C782AD82FEC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E79B73C4-56A6-4E31-8B3E-AD91008E5740}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -118,7 +118,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="106">
   <si>
     <t>https://www.facebook.com/groups/914953618536575/posts/6742148269150385/</t>
   </si>
@@ -433,6 +433,9 @@
   </si>
   <si>
     <t>https://github.com/theguyben/Rentalytics/blob/main/posts_screenshots/Hedia_Leshem.png?raw=true</t>
+  </si>
+  <si>
+    <t>(שרן)</t>
   </si>
 </sst>
 </file>
@@ -860,8 +863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="R36" sqref="R36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2483,9 +2486,8 @@
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="P25" s="10" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="P25" s="10" t="s">
+        <v>105</v>
       </c>
       <c r="Q25" s="10" t="e">
         <f>NA()</f>

</xml_diff>

<commit_message>
Updated data and map
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\97254\Desktop\Guy\Projects\Rentalytics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E79B73C4-56A6-4E31-8B3E-AD91008E5740}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10415EB2-C683-44B7-A93F-97F94CA06523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -118,7 +118,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="105">
   <si>
     <t>https://www.facebook.com/groups/914953618536575/posts/6742148269150385/</t>
   </si>
@@ -433,9 +433,6 @@
   </si>
   <si>
     <t>https://github.com/theguyben/Rentalytics/blob/main/posts_screenshots/Hedia_Leshem.png?raw=true</t>
-  </si>
-  <si>
-    <t>(שרן)</t>
   </si>
 </sst>
 </file>
@@ -2445,21 +2442,20 @@
       <c r="D25" s="1">
         <v>3</v>
       </c>
-      <c r="E25" s="1" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F25" s="1" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G25" s="1" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H25" s="1" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="E25" s="1">
+        <v>3</v>
+      </c>
+      <c r="F25" s="1" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="G25" s="1" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H25" s="1" t="b">
+        <f>FALSE</f>
+        <v>0</v>
       </c>
       <c r="I25" s="1" t="e">
         <f>NA()</f>
@@ -2482,12 +2478,13 @@
       <c r="N25" s="2">
         <v>45121</v>
       </c>
-      <c r="O25" s="1" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P25" s="10" t="s">
-        <v>105</v>
+      <c r="O25" s="1" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="P25" s="10" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
       </c>
       <c r="Q25" s="10" t="e">
         <f>NA()</f>

</xml_diff>